<commit_message>
Simplify template schema structure
</commit_message>
<xml_diff>
--- a/manifest_examples/pbmc.xlsx
+++ b/manifest_examples/pbmc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/manifest_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7189AD32-F713-534E-97A7-795F77318411}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C569824-0897-C941-B497-3121CD5E4DC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41040" yWindow="2320" windowWidth="22600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="460" windowWidth="26820" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CORE_DATA" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -264,7 +264,267 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Trial Participant Identifier. Example: PT123.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date of blood collection.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time of blood collection.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date of blood processing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time of blood processing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sample location within the shipping container. Example: A1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of sample sent.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The format in which the sample was sent.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quantity of each sample shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Volume of sample shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Volume units. Example: ml.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -272,12 +532,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
+    <comment ref="W22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -285,12 +545,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
+    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -298,12 +558,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
+    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -311,7 +571,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="Z22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -324,12 +584,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
+    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -337,276 +597,16 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
+    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Status of sample used for other assay, exhausted, destroyed, or returned.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Trial Participant Identifier. Example: PT123.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Date of blood collection.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Time of blood collection.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Date of blood processing.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Time of blood processing.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sample location within the shipping container. Example: A1.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Type of sample sent.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The format in which the sample was sent.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Quantity of each sample shipped.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Volume of sample shipped.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Volume units. Example: ml.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
         </r>
       </text>
     </comment>
@@ -692,6 +692,63 @@
     <t>#d</t>
   </si>
   <si>
+    <t>TRIAL PARTICIPANT ID</t>
+  </si>
+  <si>
+    <t>CIMAC PARTICIPANT ID</t>
+  </si>
+  <si>
+    <t>COHORT ID</t>
+  </si>
+  <si>
+    <t>ARM ID</t>
+  </si>
+  <si>
+    <t>SITE SAMPLE ID</t>
+  </si>
+  <si>
+    <t>CIMAC SAMPLE ID</t>
+  </si>
+  <si>
+    <t>TIME POINT</t>
+  </si>
+  <si>
+    <t>BLOOD COLLECTION DATE</t>
+  </si>
+  <si>
+    <t>BLOOD COLLECTION TIME</t>
+  </si>
+  <si>
+    <t>BLOOD PROCESSING DATE</t>
+  </si>
+  <si>
+    <t>BLOOD PROCESSING TIME</t>
+  </si>
+  <si>
+    <t>SAMPLE LOCATION</t>
+  </si>
+  <si>
+    <t>SPECIMEN TYPE</t>
+  </si>
+  <si>
+    <t>SPECIMEN FORMAT</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>VOLUME QUANTITY</t>
+  </si>
+  <si>
+    <t>VOLUME UNITS</t>
+  </si>
+  <si>
+    <t>PBMC ALIQUOTED</t>
+  </si>
+  <si>
+    <t>SAMPLE SOURCE</t>
+  </si>
+  <si>
     <t>CIMAC ALIQUOT ID</t>
   </si>
   <si>
@@ -713,61 +770,46 @@
     <t>SAMPLE STATUS</t>
   </si>
   <si>
-    <t>TRIAL PARTICIPANT ID</t>
-  </si>
-  <si>
-    <t>CIMAC PARTICIPANT ID</t>
-  </si>
-  <si>
-    <t>COHORT ID</t>
-  </si>
-  <si>
-    <t>ARM ID</t>
-  </si>
-  <si>
-    <t>SITE SAMPLE ID</t>
-  </si>
-  <si>
-    <t>CIMAC SAMPLE ID</t>
-  </si>
-  <si>
-    <t>TIME POINT</t>
-  </si>
-  <si>
-    <t>BLOOD COLLECTION DATE</t>
-  </si>
-  <si>
-    <t>BLOOD COLLECTION TIME</t>
-  </si>
-  <si>
-    <t>BLOOD PROCESSING DATE</t>
-  </si>
-  <si>
-    <t>BLOOD PROCESSING TIME</t>
-  </si>
-  <si>
-    <t>SAMPLE LOCATION</t>
-  </si>
-  <si>
-    <t>SPECIMEN TYPE</t>
-  </si>
-  <si>
-    <t>SPECIMEN FORMAT</t>
-  </si>
-  <si>
-    <t>QUANTITY</t>
-  </si>
-  <si>
-    <t>VOLUME QUANTITY</t>
-  </si>
-  <si>
-    <t>VOLUME UNITS</t>
-  </si>
-  <si>
-    <t>PBMC ALIQUOTED</t>
-  </si>
-  <si>
-    <t>SAMPLE SOURCE</t>
+    <t>CIMAC-12345</t>
+  </si>
+  <si>
+    <t>CIMAC-45678</t>
+  </si>
+  <si>
+    <t>CIMAC-54321</t>
+  </si>
+  <si>
+    <t>CIMAC-12354</t>
+  </si>
+  <si>
+    <t>CIMAC-12435</t>
+  </si>
+  <si>
+    <t>CIMAC-14345</t>
+  </si>
+  <si>
+    <t>Usable for Assay</t>
+  </si>
+  <si>
+    <t>Replacement Tested</t>
+  </si>
+  <si>
+    <t>Sample Exhausted</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>PBMC</t>
+  </si>
+  <si>
+    <t>EDTA Tube</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>FFPE block #52</t>
   </si>
   <si>
     <t>R123</t>
@@ -795,55 +837,13 @@
   </si>
   <si>
     <t>DFCI</t>
-  </si>
-  <si>
-    <t>Usable for Assay</t>
-  </si>
-  <si>
-    <t>Replacement Tested</t>
-  </si>
-  <si>
-    <t>Sample Exhausted</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>PBMC</t>
-  </si>
-  <si>
-    <t>EDTA Tube</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>FFPE block #52</t>
-  </si>
-  <si>
-    <t>CIMAC-12345</t>
-  </si>
-  <si>
-    <t>CIMAC-45678</t>
-  </si>
-  <si>
-    <t>CIMAC-54321</t>
-  </si>
-  <si>
-    <t>CIMAC-12354</t>
-  </si>
-  <si>
-    <t>CIMAC-12435</t>
-  </si>
-  <si>
-    <t>CIMAC-14345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,12 +862,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -944,14 +938,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1293,7 +1287,7 @@
   <dimension ref="A1:AB222"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1306,35 +1300,35 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
     </row>
     <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1416,7 +1410,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1444,7 +1438,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1452,7 +1446,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1480,7 +1474,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1488,7 +1482,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1516,7 +1510,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1632,7 +1626,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1668,7 +1662,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1704,7 +1698,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1740,7 +1734,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1775,7 +1769,7 @@
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="6">
         <v>41590</v>
       </c>
       <c r="D14" s="1"/>
@@ -1920,7 +1914,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1956,7 +1950,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1985,65 +1979,65 @@
       <c r="AB19" s="1"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>32</v>
@@ -2107,516 +2101,516 @@
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
-        <v>68</v>
+      <c r="B23">
+        <v>12345</v>
       </c>
       <c r="C23">
+        <v>54321</v>
+      </c>
+      <c r="D23">
+        <v>12345</v>
+      </c>
+      <c r="E23">
+        <v>54321</v>
+      </c>
+      <c r="F23">
+        <v>12345</v>
+      </c>
+      <c r="G23">
+        <v>54321</v>
+      </c>
+      <c r="H23">
+        <v>12345</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="J23" s="4">
+        <v>41193</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="L23" s="4">
+        <v>41193</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="N23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O23" t="s">
+        <v>61</v>
+      </c>
+      <c r="P23" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q23">
+        <v>100</v>
+      </c>
+      <c r="R23">
+        <v>100</v>
+      </c>
+      <c r="S23" t="s">
+        <v>63</v>
+      </c>
+      <c r="T23">
+        <v>10</v>
+      </c>
+      <c r="U23" t="s">
+        <v>64</v>
+      </c>
+      <c r="V23" t="s">
+        <v>51</v>
+      </c>
+      <c r="W23">
         <v>123</v>
       </c>
-      <c r="D23">
+      <c r="X23">
         <v>122</v>
-      </c>
-      <c r="E23">
-        <v>100</v>
-      </c>
-      <c r="F23" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" t="s">
-        <v>61</v>
-      </c>
-      <c r="H23" t="s">
-        <v>62</v>
-      </c>
-      <c r="I23">
-        <v>12345</v>
-      </c>
-      <c r="J23">
-        <v>54321</v>
-      </c>
-      <c r="K23">
-        <v>12345</v>
-      </c>
-      <c r="L23">
-        <v>54321</v>
-      </c>
-      <c r="M23">
-        <v>12345</v>
-      </c>
-      <c r="N23">
-        <v>54321</v>
-      </c>
-      <c r="O23">
-        <v>12345</v>
-      </c>
-      <c r="P23" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="Q23" s="6">
-        <v>41193</v>
-      </c>
-      <c r="R23" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="S23" s="6">
-        <v>41193</v>
-      </c>
-      <c r="T23" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="U23" t="s">
-        <v>63</v>
-      </c>
-      <c r="V23" t="s">
-        <v>64</v>
-      </c>
-      <c r="W23" t="s">
-        <v>65</v>
-      </c>
-      <c r="X23">
-        <v>100</v>
       </c>
       <c r="Y23">
         <v>100</v>
       </c>
       <c r="Z23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA23">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>58</v>
       </c>
       <c r="AB23" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
-        <v>69</v>
+      <c r="B24">
+        <v>12345</v>
       </c>
       <c r="C24">
+        <v>54321</v>
+      </c>
+      <c r="D24">
+        <v>12345</v>
+      </c>
+      <c r="E24">
+        <v>54321</v>
+      </c>
+      <c r="F24">
+        <v>12345</v>
+      </c>
+      <c r="G24">
+        <v>54321</v>
+      </c>
+      <c r="H24">
+        <v>12345</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="J24" s="4">
+        <v>41193</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="L24" s="4">
+        <v>41193</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="N24" t="s">
+        <v>60</v>
+      </c>
+      <c r="O24" t="s">
+        <v>61</v>
+      </c>
+      <c r="P24" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q24">
+        <v>100</v>
+      </c>
+      <c r="R24">
+        <v>100</v>
+      </c>
+      <c r="S24" t="s">
+        <v>63</v>
+      </c>
+      <c r="T24">
+        <v>10</v>
+      </c>
+      <c r="U24" t="s">
+        <v>64</v>
+      </c>
+      <c r="V24" t="s">
+        <v>52</v>
+      </c>
+      <c r="W24">
         <v>123</v>
       </c>
-      <c r="D24">
+      <c r="X24">
         <v>122</v>
-      </c>
-      <c r="E24">
-        <v>100</v>
-      </c>
-      <c r="F24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G24" t="s">
-        <v>61</v>
-      </c>
-      <c r="H24" t="s">
-        <v>62</v>
-      </c>
-      <c r="I24">
-        <v>12345</v>
-      </c>
-      <c r="J24">
-        <v>54321</v>
-      </c>
-      <c r="K24">
-        <v>12345</v>
-      </c>
-      <c r="L24">
-        <v>54321</v>
-      </c>
-      <c r="M24">
-        <v>12345</v>
-      </c>
-      <c r="N24">
-        <v>54321</v>
-      </c>
-      <c r="O24">
-        <v>12345</v>
-      </c>
-      <c r="P24" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="Q24" s="6">
-        <v>41193</v>
-      </c>
-      <c r="R24" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="S24" s="6">
-        <v>41193</v>
-      </c>
-      <c r="T24" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="U24" t="s">
-        <v>63</v>
-      </c>
-      <c r="V24" t="s">
-        <v>64</v>
-      </c>
-      <c r="W24" t="s">
-        <v>65</v>
-      </c>
-      <c r="X24">
-        <v>100</v>
       </c>
       <c r="Y24">
         <v>100</v>
       </c>
       <c r="Z24" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA24">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>58</v>
       </c>
       <c r="AB24" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>70</v>
+      <c r="B25">
+        <v>12345</v>
       </c>
       <c r="C25">
+        <v>54321</v>
+      </c>
+      <c r="D25">
+        <v>12345</v>
+      </c>
+      <c r="E25">
+        <v>54321</v>
+      </c>
+      <c r="F25">
+        <v>12345</v>
+      </c>
+      <c r="G25">
+        <v>54321</v>
+      </c>
+      <c r="H25">
+        <v>12345</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="J25" s="4">
+        <v>41193</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="L25" s="4">
+        <v>41193</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="N25" t="s">
+        <v>60</v>
+      </c>
+      <c r="O25" t="s">
+        <v>61</v>
+      </c>
+      <c r="P25" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q25">
+        <v>100</v>
+      </c>
+      <c r="R25">
+        <v>100</v>
+      </c>
+      <c r="S25" t="s">
+        <v>63</v>
+      </c>
+      <c r="T25">
+        <v>10</v>
+      </c>
+      <c r="U25" t="s">
+        <v>64</v>
+      </c>
+      <c r="V25" t="s">
+        <v>53</v>
+      </c>
+      <c r="W25">
         <v>123</v>
       </c>
-      <c r="D25">
+      <c r="X25">
         <v>122</v>
-      </c>
-      <c r="E25">
-        <v>100</v>
-      </c>
-      <c r="F25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25">
-        <v>12345</v>
-      </c>
-      <c r="J25">
-        <v>54321</v>
-      </c>
-      <c r="K25">
-        <v>12345</v>
-      </c>
-      <c r="L25">
-        <v>54321</v>
-      </c>
-      <c r="M25">
-        <v>12345</v>
-      </c>
-      <c r="N25">
-        <v>54321</v>
-      </c>
-      <c r="O25">
-        <v>12345</v>
-      </c>
-      <c r="P25" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="Q25" s="6">
-        <v>41193</v>
-      </c>
-      <c r="R25" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="S25" s="6">
-        <v>41193</v>
-      </c>
-      <c r="T25" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="U25" t="s">
-        <v>63</v>
-      </c>
-      <c r="V25" t="s">
-        <v>64</v>
-      </c>
-      <c r="W25" t="s">
-        <v>65</v>
-      </c>
-      <c r="X25">
-        <v>100</v>
       </c>
       <c r="Y25">
         <v>100</v>
       </c>
       <c r="Z25" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA25">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>58</v>
       </c>
       <c r="AB25" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>71</v>
+      <c r="B26">
+        <v>12345</v>
       </c>
       <c r="C26">
+        <v>54321</v>
+      </c>
+      <c r="D26">
+        <v>12345</v>
+      </c>
+      <c r="E26">
+        <v>54321</v>
+      </c>
+      <c r="F26">
+        <v>12345</v>
+      </c>
+      <c r="G26">
+        <v>54321</v>
+      </c>
+      <c r="H26">
+        <v>12345</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="J26" s="4">
+        <v>41193</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="L26" s="4">
+        <v>41193</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="N26" t="s">
+        <v>60</v>
+      </c>
+      <c r="O26" t="s">
+        <v>61</v>
+      </c>
+      <c r="P26" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q26">
+        <v>100</v>
+      </c>
+      <c r="R26">
+        <v>100</v>
+      </c>
+      <c r="S26" t="s">
+        <v>63</v>
+      </c>
+      <c r="T26">
+        <v>10</v>
+      </c>
+      <c r="U26" t="s">
+        <v>64</v>
+      </c>
+      <c r="V26" t="s">
+        <v>54</v>
+      </c>
+      <c r="W26">
         <v>123</v>
       </c>
-      <c r="D26">
+      <c r="X26">
         <v>122</v>
-      </c>
-      <c r="E26">
-        <v>100</v>
-      </c>
-      <c r="F26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" t="s">
-        <v>62</v>
-      </c>
-      <c r="I26">
-        <v>12345</v>
-      </c>
-      <c r="J26">
-        <v>54321</v>
-      </c>
-      <c r="K26">
-        <v>12345</v>
-      </c>
-      <c r="L26">
-        <v>54321</v>
-      </c>
-      <c r="M26">
-        <v>12345</v>
-      </c>
-      <c r="N26">
-        <v>54321</v>
-      </c>
-      <c r="O26">
-        <v>12345</v>
-      </c>
-      <c r="P26" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="Q26" s="6">
-        <v>41193</v>
-      </c>
-      <c r="R26" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="S26" s="6">
-        <v>41193</v>
-      </c>
-      <c r="T26" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="U26" t="s">
-        <v>63</v>
-      </c>
-      <c r="V26" t="s">
-        <v>64</v>
-      </c>
-      <c r="W26" t="s">
-        <v>65</v>
-      </c>
-      <c r="X26">
-        <v>100</v>
       </c>
       <c r="Y26">
         <v>100</v>
       </c>
       <c r="Z26" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA26">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>58</v>
       </c>
       <c r="AB26" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
-        <v>72</v>
+      <c r="B27">
+        <v>12345</v>
       </c>
       <c r="C27">
+        <v>54321</v>
+      </c>
+      <c r="D27">
+        <v>12345</v>
+      </c>
+      <c r="E27">
+        <v>54321</v>
+      </c>
+      <c r="F27">
+        <v>12345</v>
+      </c>
+      <c r="G27">
+        <v>54321</v>
+      </c>
+      <c r="H27">
+        <v>12345</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="J27" s="4">
+        <v>41193</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="L27" s="4">
+        <v>41193</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="N27" t="s">
+        <v>60</v>
+      </c>
+      <c r="O27" t="s">
+        <v>61</v>
+      </c>
+      <c r="P27" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q27">
+        <v>100</v>
+      </c>
+      <c r="R27">
+        <v>100</v>
+      </c>
+      <c r="S27" t="s">
+        <v>63</v>
+      </c>
+      <c r="T27">
+        <v>10</v>
+      </c>
+      <c r="U27" t="s">
+        <v>64</v>
+      </c>
+      <c r="V27" t="s">
+        <v>55</v>
+      </c>
+      <c r="W27">
         <v>123</v>
       </c>
-      <c r="D27">
+      <c r="X27">
         <v>122</v>
-      </c>
-      <c r="E27">
-        <v>100</v>
-      </c>
-      <c r="F27" t="s">
-        <v>60</v>
-      </c>
-      <c r="G27" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" t="s">
-        <v>62</v>
-      </c>
-      <c r="I27">
-        <v>12345</v>
-      </c>
-      <c r="J27">
-        <v>54321</v>
-      </c>
-      <c r="K27">
-        <v>12345</v>
-      </c>
-      <c r="L27">
-        <v>54321</v>
-      </c>
-      <c r="M27">
-        <v>12345</v>
-      </c>
-      <c r="N27">
-        <v>54321</v>
-      </c>
-      <c r="O27">
-        <v>12345</v>
-      </c>
-      <c r="P27" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="Q27" s="6">
-        <v>41193</v>
-      </c>
-      <c r="R27" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="S27" s="6">
-        <v>41193</v>
-      </c>
-      <c r="T27" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="U27" t="s">
-        <v>63</v>
-      </c>
-      <c r="V27" t="s">
-        <v>64</v>
-      </c>
-      <c r="W27" t="s">
-        <v>65</v>
-      </c>
-      <c r="X27">
-        <v>100</v>
       </c>
       <c r="Y27">
         <v>100</v>
       </c>
       <c r="Z27" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA27">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>58</v>
       </c>
       <c r="AB27" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
-        <v>73</v>
+      <c r="B28">
+        <v>12345</v>
       </c>
       <c r="C28">
+        <v>54321</v>
+      </c>
+      <c r="D28">
+        <v>12345</v>
+      </c>
+      <c r="E28">
+        <v>54321</v>
+      </c>
+      <c r="F28">
+        <v>12345</v>
+      </c>
+      <c r="G28">
+        <v>54321</v>
+      </c>
+      <c r="H28">
+        <v>12345</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="J28" s="4">
+        <v>41193</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="L28" s="4">
+        <v>41193</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.42444444444444446</v>
+      </c>
+      <c r="N28" t="s">
+        <v>60</v>
+      </c>
+      <c r="O28" t="s">
+        <v>61</v>
+      </c>
+      <c r="P28" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q28">
+        <v>100</v>
+      </c>
+      <c r="R28">
+        <v>100</v>
+      </c>
+      <c r="S28" t="s">
+        <v>63</v>
+      </c>
+      <c r="T28">
+        <v>10</v>
+      </c>
+      <c r="U28" t="s">
+        <v>64</v>
+      </c>
+      <c r="V28" t="s">
+        <v>56</v>
+      </c>
+      <c r="W28">
         <v>123</v>
       </c>
-      <c r="D28">
+      <c r="X28">
         <v>122</v>
-      </c>
-      <c r="E28">
-        <v>100</v>
-      </c>
-      <c r="F28" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28" t="s">
-        <v>61</v>
-      </c>
-      <c r="H28" t="s">
-        <v>62</v>
-      </c>
-      <c r="I28">
-        <v>12345</v>
-      </c>
-      <c r="J28">
-        <v>54321</v>
-      </c>
-      <c r="K28">
-        <v>12345</v>
-      </c>
-      <c r="L28">
-        <v>54321</v>
-      </c>
-      <c r="M28">
-        <v>12345</v>
-      </c>
-      <c r="N28">
-        <v>54321</v>
-      </c>
-      <c r="O28">
-        <v>12345</v>
-      </c>
-      <c r="P28" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="Q28" s="6">
-        <v>41193</v>
-      </c>
-      <c r="R28" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="S28" s="6">
-        <v>41193</v>
-      </c>
-      <c r="T28" s="5">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="U28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V28" t="s">
-        <v>64</v>
-      </c>
-      <c r="W28" t="s">
-        <v>65</v>
-      </c>
-      <c r="X28">
-        <v>100</v>
       </c>
       <c r="Y28">
         <v>100</v>
       </c>
       <c r="Z28" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA28">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>58</v>
       </c>
       <c r="AB28" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
@@ -3596,39 +3590,39 @@
     <mergeCell ref="V21:AB21"/>
   </mergeCells>
   <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{548917DF-2E1F-5A49-8FC5-E31A3D19828B}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{94C15CD1-BE06-8F43-9426-D85803359AA7}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{270FB13E-DC99-8E48-BDAE-981C5C4F51B7}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{1CBBEC43-9C26-174F-BDB0-FC3D9B3C3B77}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23:F222" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L23:L222 J23:J222" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>AND(ISNUMBER(J23:J222),LEFT(CELL("format",J23:J222),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23:G222" xr:uid="{00000000-0002-0000-0000-000005000000}">
-      <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H23:H222" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="S23:S222 Q23:Q222" xr:uid="{00000000-0002-0000-0000-000007000000}">
-      <formula1>AND(ISNUMBER(Q23:Q222),LEFT(CELL("format",Q23:Q222),1)="D")</formula1>
-    </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="T23:T222 R23:R222" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M23:M222 K23:K222" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V23:V222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W23:W222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P23:P222" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Other,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+      <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+      <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB23:AB222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>